<commit_message>
Initial commit with necessary files
</commit_message>
<xml_diff>
--- a/conditions.xlsx
+++ b/conditions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gau20/Desktop/stage programmation/N-back HDG/n1-back/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gau20/Desktop/stage programmation/N-back HDG/condition 1/n1-back/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66119077-D824-654C-AAAB-A76250F57699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E63B135-CA7E-714A-A975-DBB2D147F50F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2000" yWindow="500" windowWidth="16300" windowHeight="11900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11340" yWindow="500" windowWidth="16300" windowHeight="11900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -436,7 +436,7 @@
   <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -498,10 +498,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -512,10 +512,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -582,10 +582,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -599,7 +599,7 @@
         <v>6</v>
       </c>
       <c r="C12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -918,10 +918,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -988,10 +988,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C40" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>

</xml_diff>